<commit_message>
hardware: outputs: Updating main outputs #47
</commit_message>
<xml_diff>
--- a/hardware/outputs/board_bom/board_bom.xlsx
+++ b/hardware/outputs/board_bom/board_bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yan Azeredo\Desktop\SpaceLab\ttc2\hardware\outputs\board_bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F871939-759A-4B85-9C15-AE9A88C8F3C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E82C857-040E-44C0-B7CA-C54585EE98FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,10 +73,10 @@
     <t>TTC2</t>
   </si>
   <si>
-    <t>6/3/2021</t>
-  </si>
-  <si>
-    <t>2:46:30 PM</t>
+    <t>6/15/2021</t>
+  </si>
+  <si>
+    <t>5:23:06 PM</t>
   </si>
   <si>
     <t>Designator</t>
@@ -926,8 +926,8 @@
       <xdr:rowOff>191767</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1866900</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>88991</xdr:rowOff>
     </xdr:to>
@@ -1246,7 +1246,7 @@
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.140625" style="3" bestFit="1" customWidth="1"/>
@@ -1382,11 +1382,11 @@
       </c>
       <c r="E7" s="7">
         <f ca="1">TODAY()</f>
-        <v>44350</v>
+        <v>44362</v>
       </c>
       <c r="F7" s="8">
         <f ca="1">NOW()</f>
-        <v>44350.616906365743</v>
+        <v>44362.72703587963</v>
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="20"/>
@@ -2152,7 +2152,7 @@
         <v>52</v>
       </c>
       <c r="F32" s="25" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="G32" s="26" t="s">
         <v>104</v>
@@ -2703,7 +2703,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="64" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="68" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>